<commit_message>
train without label and CV for feature selection
</commit_message>
<xml_diff>
--- a/network-attack-detection/output/ctu_13/results/sum_files_results.xlsx
+++ b/network-attack-detection/output/ctu_13/results/sum_files_results.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="1544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="1547">
   <si>
     <t xml:space="preserve">Algorithm</t>
   </si>
@@ -4608,7 +4608,13 @@
     <t xml:space="preserve">MS-MCD</t>
   </si>
   <si>
-    <t xml:space="preserve">RPCA</t>
+    <t xml:space="preserve">RPCA_reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skew-RPCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skew-RPCA_reg</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -4666,6 +4672,9 @@
   </si>
   <si>
     <t xml:space="preserve">nsys.ay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average F1</t>
   </si>
 </sst>
 </file>
@@ -4678,7 +4687,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4709,15 +4718,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE181E"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="17">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4733,13 +4735,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFF2DCDB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2DCDB"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFCD5B5"/>
       </patternFill>
     </fill>
     <fill>
@@ -4762,56 +4764,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFF2DCDB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF999999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF999999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFBCC"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0EFD4"/>
-        <bgColor rgb="FFD7E4BD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF37B70"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -4849,7 +4803,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4910,39 +4864,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4950,39 +4884,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4990,20 +4892,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5018,11 +4908,11 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF2DCDB"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -5033,12 +4923,12 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFBCC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFF2DCDB"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFF37B70"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFB9CDE5"/>
       <rgbColor rgb="FF000080"/>
@@ -5050,8 +4940,8 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFD7E4BD"/>
-      <rgbColor rgb="FFE0EFD4"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FFB7DEE8"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -5063,8 +4953,8 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666666"/>
-      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -17410,10 +17300,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AS16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH8" activeCellId="0" sqref="AH8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17421,8 +17311,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="4" style="0" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="4" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="12" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="16" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="20" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="33" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="37" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="41" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="44" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17431,159 +17330,195 @@
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>1519</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
         <v>1520</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="20" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15" t="s">
         <v>1521</v>
       </c>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="21" t="s">
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15" t="s">
         <v>1522</v>
       </c>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="22" t="s">
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15" t="s">
         <v>1523</v>
       </c>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15" t="s">
         <v>1524</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15" t="s">
+        <v>1525</v>
+      </c>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>1526</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="A2" s="16" t="s">
         <v>1527</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="17" t="s">
         <v>1528</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="18" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>1528</v>
-      </c>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="J2" s="26" t="n">
+      <c r="J2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="26" t="n">
+      <c r="K2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="27" t="s">
-        <v>1528</v>
-      </c>
-      <c r="M2" s="27" t="s">
+      <c r="L2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="M2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="N2" s="27" t="n">
+      <c r="N2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="27" t="n">
+      <c r="O2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="P2" s="28" t="s">
-        <v>1528</v>
-      </c>
-      <c r="Q2" s="28" t="s">
+      <c r="P2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="R2" s="28" t="n">
+      <c r="R2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="S2" s="28" t="n">
+      <c r="S2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="T2" s="29" t="s">
-        <v>1528</v>
-      </c>
-      <c r="U2" s="29" t="s">
+      <c r="T2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="U2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="V2" s="29" t="n">
+      <c r="V2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="29" t="n">
+      <c r="W2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="30" t="s">
-        <v>1528</v>
-      </c>
-      <c r="Y2" s="30" t="s">
+      <c r="X2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="Y2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="Z2" s="30" t="n">
+      <c r="Z2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="AA2" s="30" t="n">
+      <c r="AA2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="AB2" s="31" t="s">
-        <v>1528</v>
-      </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AB2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="AC2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="AD2" s="31" t="n">
+      <c r="AD2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="AE2" s="31" t="n">
+      <c r="AE2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="AF2" s="32" t="s">
-        <v>1528</v>
-      </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AF2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="AG2" s="16" t="s">
         <v>903</v>
       </c>
-      <c r="AH2" s="32" t="n">
+      <c r="AH2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="AI2" s="32" t="n">
+      <c r="AI2" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="AK2" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="AL2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN2" s="16" t="s">
+        <v>1530</v>
+      </c>
+      <c r="AO2" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="AP2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="16" t="n">
         <v>2</v>
       </c>
     </row>
@@ -17591,1392 +17526,1935 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>1529</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>1530</v>
-      </c>
-      <c r="D3" s="33" t="n">
+      <c r="B3" s="19" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D3" s="20" t="n">
         <v>0.705633713961264</v>
       </c>
-      <c r="E3" s="34" t="n">
+      <c r="E3" s="20" t="n">
         <v>0.026263670024972</v>
       </c>
-      <c r="F3" s="35" t="n">
+      <c r="F3" s="20" t="n">
         <v>0.455016404766016</v>
       </c>
-      <c r="G3" s="35" t="n">
+      <c r="G3" s="20" t="n">
         <v>0.598124604850822</v>
       </c>
-      <c r="H3" s="34" t="n">
+      <c r="H3" s="20" t="n">
         <v>0.66084158728156</v>
       </c>
-      <c r="I3" s="34" t="n">
+      <c r="I3" s="20" t="n">
         <v>0.0204946996466431</v>
       </c>
-      <c r="J3" s="35" t="n">
+      <c r="J3" s="20" t="n">
         <v>0.407414072341191</v>
       </c>
-      <c r="K3" s="35" t="n">
+      <c r="K3" s="20" t="n">
         <v>0.278280542986425</v>
       </c>
-      <c r="L3" s="34" t="n">
+      <c r="L3" s="20" t="n">
         <v>0.661346287300486</v>
       </c>
-      <c r="M3" s="34" t="n">
+      <c r="M3" s="20" t="n">
         <v>0.0167631464648204</v>
       </c>
-      <c r="N3" s="35" t="n">
+      <c r="N3" s="20" t="n">
         <v>0.407414072341191</v>
       </c>
-      <c r="O3" s="35" t="n">
+      <c r="O3" s="20" t="n">
         <v>0.278280542986425</v>
       </c>
-      <c r="P3" s="34" t="n">
+      <c r="P3" s="20" t="n">
         <v>0.342628225348558</v>
       </c>
-      <c r="Q3" s="34" t="n">
+      <c r="Q3" s="20" t="n">
         <v>0.524559688557556</v>
       </c>
-      <c r="R3" s="35" t="n">
+      <c r="R3" s="20" t="n">
         <v>0.467474278128111</v>
       </c>
-      <c r="S3" s="35" t="n">
+      <c r="S3" s="20" t="n">
         <v>0.597285067873303</v>
       </c>
-      <c r="T3" s="34" t="n">
+      <c r="T3" s="20" t="n">
         <v>0.0838712548410795</v>
       </c>
-      <c r="U3" s="34" t="n">
+      <c r="U3" s="20" t="n">
         <v>0.679649464459591</v>
       </c>
-      <c r="V3" s="35" t="n">
+      <c r="V3" s="20" t="n">
         <v>0.111211085117869</v>
       </c>
-      <c r="W3" s="35" t="n">
+      <c r="W3" s="20" t="n">
         <v>0.587194686239679</v>
       </c>
-      <c r="X3" s="34" t="n">
+      <c r="X3" s="20" t="n">
         <v>0.0838712548410795</v>
       </c>
-      <c r="Y3" s="34" t="n">
+      <c r="Y3" s="20" t="n">
         <v>0.679472426307869</v>
       </c>
-      <c r="Z3" s="35" t="n">
+      <c r="Z3" s="20" t="n">
         <v>0.111211085117869</v>
       </c>
-      <c r="AA3" s="35" t="n">
+      <c r="AA3" s="20" t="n">
         <v>0.587194686239679</v>
       </c>
-      <c r="AB3" s="34" t="n">
+      <c r="AB3" s="20" t="n">
         <v>0.0690808150905306</v>
       </c>
-      <c r="AC3" s="34" t="n">
+      <c r="AC3" s="20" t="n">
         <v>0.517039812015874</v>
       </c>
-      <c r="AD3" s="35" t="n">
+      <c r="AD3" s="20" t="n">
         <v>0.103113190570452</v>
       </c>
-      <c r="AE3" s="35" t="n">
+      <c r="AE3" s="20" t="n">
         <v>0.335896309314587</v>
       </c>
-      <c r="AF3" s="33" t="n">
+      <c r="AF3" s="20" t="n">
         <v>0.925207</v>
       </c>
-      <c r="AG3" s="36" t="n">
+      <c r="AG3" s="20" t="n">
         <v>0.92665</v>
       </c>
-      <c r="AH3" s="37" t="n">
+      <c r="AH3" s="20" t="n">
         <v>0.808038</v>
       </c>
-      <c r="AI3" s="35" t="n">
+      <c r="AI3" s="20" t="n">
         <v>0.670103</v>
+      </c>
+      <c r="AJ3" s="20" t="n">
+        <v>0.975751</v>
+      </c>
+      <c r="AK3" s="20" t="n">
+        <v>0.977356</v>
+      </c>
+      <c r="AL3" s="20" t="n">
+        <v>0.797976</v>
+      </c>
+      <c r="AM3" s="20" t="n">
+        <v>0.726804</v>
+      </c>
+      <c r="AN3" s="20" t="n">
+        <v>0.99367</v>
+      </c>
+      <c r="AO3" s="20" t="n">
+        <v>0.998968</v>
+      </c>
+      <c r="AP3" s="20" t="n">
+        <v>0.82438</v>
+      </c>
+      <c r="AQ3" s="20" t="n">
+        <v>0.222938</v>
+      </c>
+      <c r="AR3" s="21" t="n">
+        <f aca="false">MAX(D3:AQ3)</f>
+        <v>0.998968</v>
+      </c>
+      <c r="AS3" s="21" t="n">
+        <f aca="false">MAX(D3:S3)</f>
+        <v>0.705633713961264</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>1529</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>1530</v>
-      </c>
-      <c r="D4" s="34" t="n">
+      <c r="B4" s="19" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D4" s="20" t="n">
         <v>0.0256007728535201</v>
       </c>
-      <c r="E4" s="34" t="n">
+      <c r="E4" s="20" t="n">
         <v>0.53821354067893</v>
       </c>
-      <c r="F4" s="35" t="n">
+      <c r="F4" s="20" t="n">
         <v>0.189415771548336</v>
       </c>
-      <c r="G4" s="35" t="n">
+      <c r="G4" s="20" t="n">
         <v>0.16992254277729</v>
       </c>
-      <c r="H4" s="34" t="n">
+      <c r="H4" s="20" t="n">
         <v>0.00107291694807556</v>
       </c>
-      <c r="I4" s="34" t="n">
+      <c r="I4" s="20" t="n">
         <v>0.537454959226247</v>
       </c>
-      <c r="J4" s="35" t="n">
+      <c r="J4" s="20" t="n">
         <v>0.00753523536066527</v>
       </c>
-      <c r="K4" s="35" t="n">
+      <c r="K4" s="20" t="n">
         <v>0.661296818364881</v>
       </c>
-      <c r="L4" s="34" t="n">
+      <c r="L4" s="20" t="n">
         <v>0.00107291694807556</v>
       </c>
-      <c r="M4" s="34" t="n">
+      <c r="M4" s="20" t="n">
         <v>0.537454959226247</v>
       </c>
-      <c r="N4" s="35" t="n">
+      <c r="N4" s="20" t="n">
         <v>0.00753523536066527</v>
       </c>
-      <c r="O4" s="35" t="n">
+      <c r="O4" s="20" t="n">
         <v>0.661296818364881</v>
       </c>
-      <c r="P4" s="33" t="n">
+      <c r="P4" s="20" t="n">
         <v>0.711864189343293</v>
       </c>
-      <c r="Q4" s="33" t="n">
+      <c r="Q4" s="20" t="n">
         <v>0.732785723092097</v>
       </c>
-      <c r="R4" s="35" t="n">
+      <c r="R4" s="20" t="n">
         <v>0.614274039771179</v>
       </c>
-      <c r="S4" s="35" t="n">
+      <c r="S4" s="20" t="n">
         <v>0.602092828270431</v>
       </c>
-      <c r="T4" s="33" t="n">
+      <c r="T4" s="20" t="n">
         <v>0.776377356793484</v>
       </c>
-      <c r="U4" s="34" t="n">
+      <c r="U4" s="20" t="n">
         <v>0.0458941778873507</v>
       </c>
-      <c r="V4" s="35" t="n">
+      <c r="V4" s="20" t="n">
         <v>0.466765180966339</v>
       </c>
-      <c r="W4" s="35" t="n">
+      <c r="W4" s="20" t="n">
         <v>0.180826188620421</v>
       </c>
-      <c r="X4" s="33" t="n">
+      <c r="X4" s="20" t="n">
         <v>0.776377356793484</v>
       </c>
-      <c r="Y4" s="34" t="n">
+      <c r="Y4" s="20" t="n">
         <v>0.0458941778873507</v>
       </c>
-      <c r="Z4" s="35" t="n">
+      <c r="Z4" s="20" t="n">
         <v>0.466765180966339</v>
       </c>
-      <c r="AA4" s="35" t="n">
+      <c r="AA4" s="20" t="n">
         <v>0.179657053780203</v>
       </c>
-      <c r="AB4" s="34" t="n">
+      <c r="AB4" s="20" t="n">
         <v>0.693264491903309</v>
       </c>
-      <c r="AC4" s="34" t="n">
+      <c r="AC4" s="20" t="n">
         <v>0.0493077944244263</v>
       </c>
-      <c r="AD4" s="35" t="n">
+      <c r="AD4" s="20" t="n">
         <v>0.650063189295323</v>
       </c>
-      <c r="AE4" s="35" t="n">
+      <c r="AE4" s="20" t="n">
         <v>0.665865531757808</v>
       </c>
-      <c r="AF4" s="36" t="n">
+      <c r="AF4" s="20" t="n">
         <v>0.95592</v>
       </c>
-      <c r="AG4" s="33" t="n">
+      <c r="AG4" s="20" t="n">
         <v>0.941483</v>
       </c>
-      <c r="AH4" s="35" t="n">
+      <c r="AH4" s="20" t="n">
         <v>0.534075</v>
       </c>
-      <c r="AI4" s="35" t="n">
+      <c r="AI4" s="20" t="n">
         <v>0.551245</v>
+      </c>
+      <c r="AJ4" s="20" t="n">
+        <v>0.985529</v>
+      </c>
+      <c r="AK4" s="20" t="n">
+        <v>0.97757</v>
+      </c>
+      <c r="AL4" s="20" t="n">
+        <v>0.904497</v>
+      </c>
+      <c r="AM4" s="20" t="n">
+        <v>0.786681</v>
+      </c>
+      <c r="AN4" s="20" t="n">
+        <v>0.992326</v>
+      </c>
+      <c r="AO4" s="20" t="n">
+        <v>0.998315</v>
+      </c>
+      <c r="AP4" s="20" t="n">
+        <v>0.103769</v>
+      </c>
+      <c r="AQ4" s="20" t="n">
+        <v>0.347603</v>
+      </c>
+      <c r="AR4" s="21" t="n">
+        <f aca="false">MAX(D4:AQ4)</f>
+        <v>0.998315</v>
+      </c>
+      <c r="AS4" s="21" t="n">
+        <f aca="false">MAX(D4:S4)</f>
+        <v>0.732785723092097</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>1531</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D5" s="34" t="n">
+      <c r="B5" s="19" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D5" s="20" t="n">
         <v>0.190490927602153</v>
       </c>
-      <c r="E5" s="34" t="n">
+      <c r="E5" s="20" t="n">
         <v>0.022922238043969</v>
       </c>
-      <c r="F5" s="34" t="n">
+      <c r="F5" s="20" t="n">
         <v>0.051750186736135</v>
       </c>
-      <c r="G5" s="34" t="n">
+      <c r="G5" s="20" t="n">
         <v>0.175850565059688</v>
       </c>
-      <c r="H5" s="34" t="n">
+      <c r="H5" s="20" t="n">
         <v>0.198899175328634</v>
       </c>
-      <c r="I5" s="34" t="n">
+      <c r="I5" s="20" t="n">
         <v>0.0503059523642774</v>
       </c>
-      <c r="J5" s="34" t="n">
+      <c r="J5" s="20" t="n">
         <v>0.0516317215463179</v>
       </c>
-      <c r="K5" s="34" t="n">
+      <c r="K5" s="20" t="n">
         <v>0.167420835110643</v>
       </c>
-      <c r="L5" s="34" t="n">
+      <c r="L5" s="20" t="n">
         <v>0.198864605153224</v>
       </c>
-      <c r="M5" s="34" t="n">
+      <c r="M5" s="20" t="n">
         <v>0.0503059523642774</v>
       </c>
-      <c r="N5" s="34" t="n">
+      <c r="N5" s="20" t="n">
         <v>0.0516317215463179</v>
       </c>
-      <c r="O5" s="34" t="n">
+      <c r="O5" s="20" t="n">
         <v>0.167420835110643</v>
       </c>
-      <c r="P5" s="34" t="n">
+      <c r="P5" s="20" t="n">
         <v>0.0642831006362443</v>
       </c>
-      <c r="Q5" s="34" t="n">
+      <c r="Q5" s="20" t="n">
         <v>0.313041591689319</v>
       </c>
-      <c r="R5" s="34" t="n">
+      <c r="R5" s="20" t="n">
         <v>0.335717427405762</v>
       </c>
-      <c r="S5" s="34" t="n">
+      <c r="S5" s="20" t="n">
         <v>0.261747262682112</v>
       </c>
-      <c r="T5" s="34" t="n">
+      <c r="T5" s="20" t="n">
         <v>0.0450870903440594</v>
       </c>
-      <c r="U5" s="34" t="n">
+      <c r="U5" s="20" t="n">
         <v>0.320954122835859</v>
       </c>
-      <c r="V5" s="33" t="n">
+      <c r="V5" s="20" t="n">
         <v>0.61599866954931</v>
       </c>
-      <c r="W5" s="36" t="n">
+      <c r="W5" s="20" t="n">
         <v>0.639365474383981</v>
       </c>
-      <c r="X5" s="34" t="n">
+      <c r="X5" s="20" t="n">
         <v>0.0449768168967933</v>
       </c>
-      <c r="Y5" s="34" t="n">
+      <c r="Y5" s="20" t="n">
         <v>0.320954122835859</v>
       </c>
-      <c r="Z5" s="33" t="n">
+      <c r="Z5" s="20" t="n">
         <v>0.615965408282056</v>
       </c>
-      <c r="AA5" s="36" t="n">
+      <c r="AA5" s="20" t="n">
         <v>0.639365474383981</v>
       </c>
-      <c r="AB5" s="34" t="n">
+      <c r="AB5" s="20" t="n">
         <v>0.052923285255833</v>
       </c>
-      <c r="AC5" s="34" t="n">
+      <c r="AC5" s="20" t="n">
         <v>0.336531790003296</v>
       </c>
-      <c r="AD5" s="33" t="n">
+      <c r="AD5" s="20" t="n">
         <v>0.631342768381084</v>
       </c>
-      <c r="AE5" s="33" t="n">
+      <c r="AE5" s="20" t="n">
         <v>0.636702882978951</v>
       </c>
-      <c r="AF5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="0" t="n">
-        <v>0</v>
+      <c r="AF5" s="20" t="n">
+        <v>0.322275</v>
+      </c>
+      <c r="AG5" s="20" t="n">
+        <v>0.191081</v>
+      </c>
+      <c r="AH5" s="20" t="n">
+        <v>0.212555</v>
+      </c>
+      <c r="AI5" s="20" t="n">
+        <v>0.229126</v>
+      </c>
+      <c r="AJ5" s="20" t="n">
+        <v>0.000259</v>
+      </c>
+      <c r="AK5" s="20" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AL5" s="20" t="n">
+        <v>0.002571</v>
+      </c>
+      <c r="AM5" s="20" t="n">
+        <v>0.006456</v>
+      </c>
+      <c r="AN5" s="20" t="n">
+        <v>0.80941</v>
+      </c>
+      <c r="AO5" s="20" t="n">
+        <v>0.014958</v>
+      </c>
+      <c r="AP5" s="20" t="n">
+        <v>0.113001</v>
+      </c>
+      <c r="AQ5" s="20" t="n">
+        <v>0.265035</v>
+      </c>
+      <c r="AR5" s="21" t="n">
+        <f aca="false">MAX(D5:AQ5)</f>
+        <v>0.80941</v>
+      </c>
+      <c r="AS5" s="21" t="n">
+        <f aca="false">MAX(D5:S5)</f>
+        <v>0.335717427405762</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>1533</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D6" s="34" t="n">
+      <c r="B6" s="19" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="34" t="n">
+      <c r="E6" s="20" t="n">
         <v>0.00062266500622665</v>
       </c>
-      <c r="F6" s="33" t="n">
+      <c r="F6" s="20" t="n">
         <v>0.846023302938196</v>
       </c>
-      <c r="G6" s="34" t="n">
+      <c r="G6" s="20" t="n">
         <v>0.786380597014925</v>
       </c>
-      <c r="H6" s="34" t="n">
+      <c r="H6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="34" t="n">
+      <c r="I6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="33" t="n">
+      <c r="J6" s="20" t="n">
         <v>0.834562841530055</v>
       </c>
-      <c r="K6" s="34" t="n">
+      <c r="K6" s="20" t="n">
         <v>0.784028228423102</v>
       </c>
-      <c r="L6" s="34" t="n">
+      <c r="L6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="34" t="n">
+      <c r="M6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="33" t="n">
+      <c r="N6" s="20" t="n">
         <v>0.834562841530055</v>
       </c>
-      <c r="O6" s="34" t="n">
+      <c r="O6" s="20" t="n">
         <v>0.786380597014925</v>
       </c>
-      <c r="P6" s="34" t="n">
+      <c r="P6" s="20" t="n">
         <v>0.244713478611784</v>
       </c>
-      <c r="Q6" s="34" t="n">
+      <c r="Q6" s="20" t="n">
         <v>0.321668909825034</v>
       </c>
-      <c r="R6" s="34" t="n">
+      <c r="R6" s="20" t="n">
         <v>0.497599967457186</v>
       </c>
-      <c r="S6" s="34" t="n">
+      <c r="S6" s="20" t="n">
         <v>0.524879324333001</v>
       </c>
-      <c r="T6" s="34" t="n">
+      <c r="T6" s="20" t="n">
         <v>0.244713478611784</v>
       </c>
-      <c r="U6" s="34" t="n">
+      <c r="U6" s="20" t="n">
         <v>0.326962078637256</v>
       </c>
-      <c r="V6" s="34" t="n">
+      <c r="V6" s="20" t="n">
         <v>0.00546448087431694</v>
       </c>
-      <c r="W6" s="34" t="n">
+      <c r="W6" s="20" t="n">
         <v>0.0118837468754854</v>
       </c>
-      <c r="X6" s="34" t="n">
+      <c r="X6" s="20" t="n">
         <v>0.244713478611784</v>
       </c>
-      <c r="Y6" s="34" t="n">
+      <c r="Y6" s="20" t="n">
         <v>0.326962078637256</v>
       </c>
-      <c r="Z6" s="34" t="n">
+      <c r="Z6" s="20" t="n">
         <v>0.00546448087431694</v>
       </c>
-      <c r="AA6" s="34" t="n">
+      <c r="AA6" s="20" t="n">
         <v>0.0118837468754854</v>
       </c>
-      <c r="AB6" s="34" t="n">
+      <c r="AB6" s="20" t="n">
         <v>0.244713478611784</v>
       </c>
-      <c r="AC6" s="34" t="n">
+      <c r="AC6" s="20" t="n">
         <v>0.338178011677295</v>
       </c>
-      <c r="AD6" s="34" t="n">
+      <c r="AD6" s="20" t="n">
         <v>0.00546448087431694</v>
       </c>
-      <c r="AE6" s="34" t="n">
+      <c r="AE6" s="20" t="n">
         <v>0.0111482720178372</v>
       </c>
-      <c r="AF6" s="34" t="n">
+      <c r="AF6" s="20" t="n">
         <v>0.749012</v>
       </c>
-      <c r="AG6" s="34" t="n">
+      <c r="AG6" s="20" t="n">
         <v>0.729508</v>
       </c>
-      <c r="AH6" s="34" t="n">
+      <c r="AH6" s="20" t="n">
         <v>0.685567</v>
       </c>
-      <c r="AI6" s="36" t="n">
+      <c r="AI6" s="20" t="n">
         <v>0.89916</v>
+      </c>
+      <c r="AJ6" s="20" t="n">
+        <v>0.857143</v>
+      </c>
+      <c r="AK6" s="20" t="n">
+        <v>0.963758</v>
+      </c>
+      <c r="AL6" s="20" t="n">
+        <v>0.972924</v>
+      </c>
+      <c r="AM6" s="20" t="n">
+        <v>0.896703</v>
+      </c>
+      <c r="AN6" s="20" t="n">
+        <v>0.997365</v>
+      </c>
+      <c r="AO6" s="20" t="n">
+        <v>0.963758</v>
+      </c>
+      <c r="AP6" s="20" t="n">
+        <v>0.981273</v>
+      </c>
+      <c r="AQ6" s="20" t="n">
+        <v>0.988208</v>
+      </c>
+      <c r="AR6" s="21" t="n">
+        <f aca="false">MAX(D6:AQ6)</f>
+        <v>0.997365</v>
+      </c>
+      <c r="AS6" s="21" t="n">
+        <f aca="false">MAX(D6:S6)</f>
+        <v>0.846023302938196</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>1534</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>1535</v>
-      </c>
-      <c r="D7" s="34" t="n">
+      <c r="B7" s="19" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D7" s="20" t="n">
         <v>0.0356340398066095</v>
       </c>
-      <c r="E7" s="33" t="n">
+      <c r="E7" s="20" t="n">
         <v>0.851236053380004</v>
       </c>
-      <c r="F7" s="35" t="n">
+      <c r="F7" s="20" t="n">
         <v>0.772093023255814</v>
       </c>
-      <c r="G7" s="35" t="n">
+      <c r="G7" s="20" t="n">
         <v>0.58125</v>
       </c>
-      <c r="H7" s="34" t="n">
+      <c r="H7" s="20" t="n">
         <v>0.666353357476571</v>
       </c>
-      <c r="I7" s="33" t="n">
+      <c r="I7" s="20" t="n">
         <v>0.862385321100917</v>
       </c>
-      <c r="J7" s="35" t="n">
+      <c r="J7" s="20" t="n">
         <v>0.818791946308725</v>
       </c>
-      <c r="K7" s="35" t="n">
+      <c r="K7" s="20" t="n">
         <v>0.612121212121212</v>
       </c>
-      <c r="L7" s="34" t="n">
+      <c r="L7" s="20" t="n">
         <v>0.66179962341464</v>
       </c>
-      <c r="M7" s="33" t="n">
+      <c r="M7" s="20" t="n">
         <v>0.862385321100917</v>
       </c>
-      <c r="N7" s="35" t="n">
+      <c r="N7" s="20" t="n">
         <v>0.814568386947466</v>
       </c>
-      <c r="O7" s="35" t="n">
+      <c r="O7" s="20" t="n">
         <v>0.606256109481916</v>
       </c>
-      <c r="P7" s="34" t="n">
+      <c r="P7" s="20" t="n">
         <v>0.362965868450644</v>
       </c>
-      <c r="Q7" s="34" t="n">
+      <c r="Q7" s="20" t="n">
         <v>0.275440100032314</v>
       </c>
-      <c r="R7" s="35" t="n">
+      <c r="R7" s="20" t="n">
         <v>0.665116279069767</v>
       </c>
-      <c r="S7" s="35" t="n">
+      <c r="S7" s="20" t="n">
         <v>0.4875</v>
       </c>
-      <c r="T7" s="34" t="n">
+      <c r="T7" s="20" t="n">
         <v>0.0761014686248331</v>
       </c>
-      <c r="U7" s="34" t="n">
+      <c r="U7" s="20" t="n">
         <v>0.127118644067797</v>
       </c>
-      <c r="V7" s="35" t="n">
+      <c r="V7" s="20" t="n">
         <v>0.013953488372093</v>
       </c>
-      <c r="W7" s="35" t="n">
+      <c r="W7" s="20" t="n">
         <v>0.278787878787879</v>
       </c>
-      <c r="X7" s="34" t="n">
+      <c r="X7" s="20" t="n">
         <v>0.0732683450342083</v>
       </c>
-      <c r="Y7" s="34" t="n">
+      <c r="Y7" s="20" t="n">
         <v>0.126468889530622</v>
       </c>
-      <c r="Z7" s="35" t="n">
+      <c r="Z7" s="20" t="n">
         <v>0.013953488372093</v>
       </c>
-      <c r="AA7" s="35" t="n">
+      <c r="AA7" s="20" t="n">
         <v>0.278787878787879</v>
       </c>
-      <c r="AB7" s="34" t="n">
+      <c r="AB7" s="20" t="n">
         <v>0.575807665179828</v>
       </c>
-      <c r="AC7" s="34" t="n">
+      <c r="AC7" s="20" t="n">
         <v>0.121468926553672</v>
       </c>
-      <c r="AD7" s="35" t="n">
+      <c r="AD7" s="20" t="n">
         <v>0.0142582975841048</v>
       </c>
-      <c r="AE7" s="35" t="n">
+      <c r="AE7" s="20" t="n">
         <v>0.303030303030303</v>
       </c>
-      <c r="AF7" s="34" t="n">
+      <c r="AF7" s="20" t="n">
         <v>0.400718</v>
       </c>
-      <c r="AG7" s="34" t="n">
+      <c r="AG7" s="20" t="n">
         <v>0.568745</v>
       </c>
-      <c r="AH7" s="38" t="n">
+      <c r="AH7" s="20" t="n">
         <v>0.892057</v>
       </c>
-      <c r="AI7" s="35" t="n">
+      <c r="AI7" s="20" t="n">
         <v>0.762463</v>
+      </c>
+      <c r="AJ7" s="20" t="n">
+        <v>0.945626</v>
+      </c>
+      <c r="AK7" s="20" t="n">
+        <v>0.944584</v>
+      </c>
+      <c r="AL7" s="20" t="n">
+        <v>0.822811</v>
+      </c>
+      <c r="AM7" s="20" t="n">
+        <v>0.621701</v>
+      </c>
+      <c r="AN7" s="20" t="n">
+        <v>0.249622</v>
+      </c>
+      <c r="AO7" s="20" t="n">
+        <v>0.929471</v>
+      </c>
+      <c r="AP7" s="20" t="n">
+        <v>0.00738</v>
+      </c>
+      <c r="AQ7" s="20" t="n">
+        <v>0.008584</v>
+      </c>
+      <c r="AR7" s="21" t="n">
+        <f aca="false">MAX(D7:AQ7)</f>
+        <v>0.945626</v>
+      </c>
+      <c r="AS7" s="21" t="n">
+        <f aca="false">MAX(D7:S7)</f>
+        <v>0.862385321100917</v>
       </c>
     </row>
     <row r="8" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>1536</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>1537</v>
-      </c>
-      <c r="D8" s="34" t="n">
+      <c r="B8" s="19" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D8" s="20" t="n">
         <v>0.000729698971272519</v>
       </c>
-      <c r="E8" s="34" t="n">
+      <c r="E8" s="20" t="n">
         <v>0.0144156425125418</v>
       </c>
-      <c r="F8" s="35" t="n">
+      <c r="F8" s="20" t="n">
         <v>0.131249090556278</v>
       </c>
-      <c r="G8" s="35" t="n">
+      <c r="G8" s="20" t="n">
         <v>0.480588721984706</v>
       </c>
-      <c r="H8" s="34" t="n">
+      <c r="H8" s="20" t="n">
         <v>0.000888303350634964</v>
       </c>
-      <c r="I8" s="34" t="n">
+      <c r="I8" s="20" t="n">
         <v>0.0144739511757201</v>
       </c>
-      <c r="J8" s="35" t="n">
+      <c r="J8" s="20" t="n">
         <v>0.131495111501703</v>
       </c>
-      <c r="K8" s="35" t="n">
+      <c r="K8" s="20" t="n">
         <v>0.478636521322141</v>
       </c>
-      <c r="L8" s="34" t="n">
+      <c r="L8" s="20" t="n">
         <v>0.000864133582181346</v>
       </c>
-      <c r="M8" s="34" t="n">
+      <c r="M8" s="20" t="n">
         <v>0.0144739511757201</v>
       </c>
-      <c r="N8" s="35" t="n">
+      <c r="N8" s="20" t="n">
         <v>0.131495111501703</v>
       </c>
-      <c r="O8" s="35" t="n">
+      <c r="O8" s="20" t="n">
         <v>0.478636521322141</v>
       </c>
-      <c r="P8" s="34" t="n">
+      <c r="P8" s="20" t="n">
         <v>0.54616327161334</v>
       </c>
-      <c r="Q8" s="34" t="n">
+      <c r="Q8" s="20" t="n">
         <v>0.478597080630213</v>
       </c>
-      <c r="R8" s="35" t="n">
+      <c r="R8" s="20" t="n">
         <v>0.482082522780792</v>
       </c>
-      <c r="S8" s="35" t="n">
+      <c r="S8" s="20" t="n">
         <v>0.537742546142925</v>
       </c>
-      <c r="T8" s="33" t="n">
+      <c r="T8" s="20" t="n">
         <v>0.668996029555912</v>
       </c>
-      <c r="U8" s="34" t="n">
+      <c r="U8" s="20" t="n">
         <v>0.534385891165709</v>
       </c>
-      <c r="V8" s="35" t="n">
+      <c r="V8" s="20" t="n">
         <v>0.56014299977651</v>
       </c>
-      <c r="W8" s="35" t="n">
+      <c r="W8" s="20" t="n">
         <v>0.568327023189777</v>
       </c>
-      <c r="X8" s="34" t="n">
+      <c r="X8" s="20" t="n">
         <v>0.669016121308492</v>
       </c>
-      <c r="Y8" s="34" t="n">
+      <c r="Y8" s="20" t="n">
         <v>0.534025482678055</v>
       </c>
-      <c r="Z8" s="35" t="n">
+      <c r="Z8" s="20" t="n">
         <v>0.56014299977651</v>
       </c>
-      <c r="AA8" s="35" t="n">
+      <c r="AA8" s="20" t="n">
         <v>0.568267865593942</v>
       </c>
-      <c r="AB8" s="33" t="n">
+      <c r="AB8" s="20" t="n">
         <v>0.669185547521798</v>
       </c>
-      <c r="AC8" s="34" t="n">
+      <c r="AC8" s="20" t="n">
         <v>0.550533386466839</v>
       </c>
-      <c r="AD8" s="35" t="n">
+      <c r="AD8" s="20" t="n">
         <v>0.560195993947152</v>
       </c>
-      <c r="AE8" s="35" t="n">
+      <c r="AE8" s="20" t="n">
         <v>0.568386180785613</v>
       </c>
-      <c r="AF8" s="33" t="n">
+      <c r="AF8" s="20" t="n">
         <v>0.678706</v>
       </c>
-      <c r="AG8" s="36" t="n">
+      <c r="AG8" s="20" t="n">
         <v>0.681629</v>
       </c>
-      <c r="AH8" s="35" t="n">
+      <c r="AH8" s="20" t="n">
         <v>0.650153</v>
       </c>
-      <c r="AI8" s="35" t="n">
+      <c r="AI8" s="20" t="n">
         <v>0.611461</v>
+      </c>
+      <c r="AJ8" s="20" t="n">
+        <v>0.955976</v>
+      </c>
+      <c r="AK8" s="20" t="n">
+        <v>0.699092</v>
+      </c>
+      <c r="AL8" s="20" t="n">
+        <v>0.124738</v>
+      </c>
+      <c r="AM8" s="20" t="n">
+        <v>0.59553</v>
+      </c>
+      <c r="AN8" s="20" t="n">
+        <v>0.96341</v>
+      </c>
+      <c r="AO8" s="20" t="n">
+        <v>0.959192</v>
+      </c>
+      <c r="AP8" s="20" t="n">
+        <v>0.772875</v>
+      </c>
+      <c r="AQ8" s="20" t="n">
+        <v>0.614212</v>
+      </c>
+      <c r="AR8" s="21" t="n">
+        <f aca="false">MAX(D8:AQ8)</f>
+        <v>0.96341</v>
+      </c>
+      <c r="AS8" s="21" t="n">
+        <f aca="false">MAX(D8:S8)</f>
+        <v>0.54616327161334</v>
       </c>
     </row>
     <row r="9" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>1538</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>1539</v>
-      </c>
-      <c r="D9" s="34" t="n">
+      <c r="B9" s="19" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D9" s="20" t="n">
         <v>0.446748185111314</v>
       </c>
-      <c r="E9" s="34" t="n">
+      <c r="E9" s="20" t="n">
         <v>0.355034065102195</v>
       </c>
-      <c r="F9" s="33" t="n">
+      <c r="F9" s="20" t="n">
         <v>0.91743119266055</v>
       </c>
-      <c r="G9" s="35" t="n">
+      <c r="G9" s="20" t="n">
         <v>0.770622212348548</v>
       </c>
-      <c r="H9" s="34" t="n">
+      <c r="H9" s="20" t="n">
         <v>0.424784625579854</v>
       </c>
-      <c r="I9" s="34" t="n">
+      <c r="I9" s="20" t="n">
         <v>0.33379158478323</v>
       </c>
-      <c r="J9" s="33" t="n">
+      <c r="J9" s="20" t="n">
         <v>0.91743119266055</v>
       </c>
-      <c r="K9" s="37" t="n">
+      <c r="K9" s="20" t="n">
         <v>0.854014598540146</v>
       </c>
-      <c r="L9" s="34" t="n">
+      <c r="L9" s="20" t="n">
         <v>0.429423459244533</v>
       </c>
-      <c r="M9" s="34" t="n">
+      <c r="M9" s="20" t="n">
         <v>0.343309744987846</v>
       </c>
-      <c r="N9" s="33" t="n">
+      <c r="N9" s="20" t="n">
         <v>0.91743119266055</v>
       </c>
-      <c r="O9" s="37" t="n">
+      <c r="O9" s="20" t="n">
         <v>0.852554744525548</v>
       </c>
-      <c r="P9" s="34" t="n">
+      <c r="P9" s="20" t="n">
         <v>0.265076209410205</v>
       </c>
-      <c r="Q9" s="34" t="n">
+      <c r="Q9" s="20" t="n">
         <v>0.408476104598738</v>
       </c>
-      <c r="R9" s="34" t="n">
+      <c r="R9" s="20" t="n">
         <v>0.603973509933775</v>
       </c>
-      <c r="S9" s="35" t="n">
+      <c r="S9" s="20" t="n">
         <v>0.613695154464454</v>
       </c>
-      <c r="T9" s="34" t="n">
+      <c r="T9" s="20" t="n">
         <v>0.0344599072233267</v>
       </c>
-      <c r="U9" s="34" t="n">
+      <c r="U9" s="20" t="n">
         <v>0.0482809085938529</v>
       </c>
-      <c r="V9" s="34" t="n">
+      <c r="V9" s="20" t="n">
         <v>0.00458715596330275</v>
       </c>
-      <c r="W9" s="35" t="n">
+      <c r="W9" s="20" t="n">
         <v>0.00746279037418278</v>
       </c>
-      <c r="X9" s="34" t="n">
+      <c r="X9" s="20" t="n">
         <v>0.0344599072233267</v>
       </c>
-      <c r="Y9" s="34" t="n">
+      <c r="Y9" s="20" t="n">
         <v>0.0499396241200446</v>
       </c>
-      <c r="Z9" s="34" t="n">
+      <c r="Z9" s="20" t="n">
         <v>0.00458715596330275</v>
       </c>
-      <c r="AA9" s="35" t="n">
+      <c r="AA9" s="20" t="n">
         <v>0.00746279037418278</v>
       </c>
-      <c r="AB9" s="34" t="n">
+      <c r="AB9" s="20" t="n">
         <v>0.0291583830351226</v>
       </c>
-      <c r="AC9" s="34" t="n">
+      <c r="AC9" s="20" t="n">
         <v>0.0360685302073941</v>
       </c>
-      <c r="AD9" s="34" t="n">
+      <c r="AD9" s="20" t="n">
         <v>0.00491400491400492</v>
       </c>
-      <c r="AE9" s="35" t="n">
+      <c r="AE9" s="20" t="n">
         <v>0.00583941605839416</v>
       </c>
-      <c r="AF9" s="34" t="n">
+      <c r="AF9" s="20" t="n">
         <v>0.46594</v>
       </c>
-      <c r="AG9" s="34" t="n">
+      <c r="AG9" s="20" t="n">
         <v>0.473907</v>
       </c>
-      <c r="AH9" s="34" t="n">
+      <c r="AH9" s="20" t="n">
         <v>0.514032</v>
       </c>
-      <c r="AI9" s="35" t="n">
+      <c r="AI9" s="20" t="n">
         <v>0.532134</v>
+      </c>
+      <c r="AJ9" s="20" t="n">
+        <v>0.013624</v>
+      </c>
+      <c r="AK9" s="20" t="n">
+        <v>0.009238</v>
+      </c>
+      <c r="AL9" s="20" t="n">
+        <v>0.006993</v>
+      </c>
+      <c r="AM9" s="20" t="n">
+        <v>0.894089</v>
+      </c>
+      <c r="AN9" s="20" t="n">
+        <v>0.009901</v>
+      </c>
+      <c r="AO9" s="20" t="n">
+        <v>0.004019</v>
+      </c>
+      <c r="AP9" s="20" t="n">
+        <v>0.057831</v>
+      </c>
+      <c r="AQ9" s="20" t="n">
+        <v>0.177096</v>
+      </c>
+      <c r="AR9" s="21" t="n">
+        <f aca="false">MAX(D9:AQ9)</f>
+        <v>0.91743119266055</v>
+      </c>
+      <c r="AS9" s="21" t="n">
+        <f aca="false">MAX(D9:S9)</f>
+        <v>0.91743119266055</v>
       </c>
     </row>
     <row r="10" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>1536</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>1540</v>
-      </c>
-      <c r="D10" s="34" t="n">
+      <c r="B10" s="19" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="34" t="n">
+      <c r="E10" s="20" t="n">
         <v>0.163115763546798</v>
       </c>
-      <c r="F10" s="34" t="n">
+      <c r="F10" s="20" t="n">
         <v>0.432432432432432</v>
       </c>
-      <c r="G10" s="33" t="n">
+      <c r="G10" s="20" t="n">
         <v>0.64</v>
       </c>
-      <c r="H10" s="34" t="n">
+      <c r="H10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="34" t="n">
+      <c r="I10" s="20" t="n">
         <v>0.196428571428571</v>
       </c>
-      <c r="J10" s="34" t="n">
+      <c r="J10" s="20" t="n">
         <v>0.4</v>
       </c>
-      <c r="K10" s="34" t="n">
+      <c r="K10" s="20" t="n">
         <v>0.48</v>
       </c>
-      <c r="L10" s="34" t="n">
+      <c r="L10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="34" t="n">
+      <c r="M10" s="20" t="n">
         <v>0.196428571428571</v>
       </c>
-      <c r="N10" s="34" t="n">
+      <c r="N10" s="20" t="n">
         <v>0.432432432432432</v>
       </c>
-      <c r="O10" s="34" t="n">
+      <c r="O10" s="20" t="n">
         <v>0.56</v>
       </c>
-      <c r="P10" s="34" t="n">
+      <c r="P10" s="20" t="n">
         <v>0.0437138900826052</v>
       </c>
-      <c r="Q10" s="34" t="n">
+      <c r="Q10" s="20" t="n">
         <v>0.0357142857142857</v>
       </c>
-      <c r="R10" s="34" t="n">
+      <c r="R10" s="20" t="n">
         <v>0.185663082437276</v>
       </c>
-      <c r="S10" s="34" t="n">
+      <c r="S10" s="20" t="n">
         <v>0.285714285714286</v>
       </c>
-      <c r="T10" s="34" t="n">
+      <c r="T10" s="20" t="n">
         <v>0.0827733966363563</v>
       </c>
-      <c r="U10" s="34" t="n">
+      <c r="U10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="V10" s="34" t="n">
+      <c r="V10" s="20" t="n">
         <v>0.0888888888888889</v>
       </c>
-      <c r="W10" s="34" t="n">
+      <c r="W10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="X10" s="34" t="n">
+      <c r="X10" s="20" t="n">
         <v>0.0827733966363563</v>
       </c>
-      <c r="Y10" s="34" t="n">
+      <c r="Y10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="Z10" s="34" t="n">
+      <c r="Z10" s="20" t="n">
         <v>0.0888888888888889</v>
       </c>
-      <c r="AA10" s="34" t="n">
+      <c r="AA10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AB10" s="34" t="n">
+      <c r="AB10" s="20" t="n">
         <v>0.0899653979238754</v>
       </c>
-      <c r="AC10" s="34" t="n">
+      <c r="AC10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AD10" s="34" t="n">
+      <c r="AD10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AE10" s="34" t="n">
+      <c r="AE10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AF10" s="34" t="n">
+      <c r="AF10" s="20" t="n">
         <v>0.071429</v>
       </c>
-      <c r="AG10" s="34" t="n">
+      <c r="AG10" s="20" t="n">
         <v>0.095238</v>
       </c>
-      <c r="AH10" s="34" t="n">
+      <c r="AH10" s="20" t="n">
         <v>0.272727</v>
       </c>
-      <c r="AI10" s="34" t="n">
+      <c r="AI10" s="20" t="n">
         <v>0.526316</v>
+      </c>
+      <c r="AJ10" s="20" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AK10" s="20" t="n">
+        <v>0.684211</v>
+      </c>
+      <c r="AL10" s="20" t="n">
+        <v>0.315789</v>
+      </c>
+      <c r="AM10" s="20" t="n">
+        <v>0.285714</v>
+      </c>
+      <c r="AN10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="21" t="n">
+        <f aca="false">MAX(D10:AQ10)</f>
+        <v>0.8</v>
+      </c>
+      <c r="AS10" s="21" t="n">
+        <f aca="false">MAX(D10:S10)</f>
+        <v>0.64</v>
       </c>
     </row>
     <row r="11" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>1541</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>1530</v>
-      </c>
-      <c r="D11" s="34" t="n">
+      <c r="B11" s="19" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D11" s="20" t="n">
         <v>0.000174200865291721</v>
       </c>
-      <c r="E11" s="34" t="n">
+      <c r="E11" s="20" t="n">
         <v>0.051928321058064</v>
       </c>
-      <c r="F11" s="34" t="n">
+      <c r="F11" s="20" t="n">
         <v>0.0356912491937218</v>
       </c>
-      <c r="G11" s="34" t="n">
+      <c r="G11" s="20" t="n">
         <v>0.050545092721675</v>
       </c>
-      <c r="H11" s="34" t="n">
+      <c r="H11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="34" t="n">
+      <c r="I11" s="20" t="n">
         <v>0.0724432830585934</v>
       </c>
-      <c r="J11" s="34" t="n">
+      <c r="J11" s="20" t="n">
         <v>0.0350462266179316</v>
       </c>
-      <c r="K11" s="34" t="n">
+      <c r="K11" s="20" t="n">
         <v>0.050545092721675</v>
       </c>
-      <c r="L11" s="34" t="n">
+      <c r="L11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M11" s="34" t="n">
+      <c r="M11" s="20" t="n">
         <v>0.0722050743877978</v>
       </c>
-      <c r="N11" s="34" t="n">
+      <c r="N11" s="20" t="n">
         <v>0.0350462266179316</v>
       </c>
-      <c r="O11" s="34" t="n">
+      <c r="O11" s="20" t="n">
         <v>0.050545092721675</v>
       </c>
-      <c r="P11" s="34" t="n">
+      <c r="P11" s="20" t="n">
         <v>0.152602175830638</v>
       </c>
-      <c r="Q11" s="34" t="n">
+      <c r="Q11" s="20" t="n">
         <v>0.0971088670632176</v>
       </c>
-      <c r="R11" s="34" t="n">
+      <c r="R11" s="20" t="n">
         <v>0.420814142033193</v>
       </c>
-      <c r="S11" s="34" t="n">
+      <c r="S11" s="20" t="n">
         <v>0.308180535966149</v>
       </c>
-      <c r="T11" s="34" t="n">
+      <c r="T11" s="20" t="n">
         <v>0.178713858424726</v>
       </c>
-      <c r="U11" s="34" t="n">
+      <c r="U11" s="20" t="n">
         <v>0.0358417820933885</v>
       </c>
-      <c r="V11" s="33" t="n">
+      <c r="V11" s="20" t="n">
         <v>0.489572135024726</v>
       </c>
-      <c r="W11" s="34" t="n">
+      <c r="W11" s="20" t="n">
         <v>0.426657263751763</v>
       </c>
-      <c r="X11" s="34" t="n">
+      <c r="X11" s="20" t="n">
         <v>0.178713858424726</v>
       </c>
-      <c r="Y11" s="34" t="n">
+      <c r="Y11" s="20" t="n">
         <v>0.0359845780379837</v>
       </c>
-      <c r="Z11" s="33" t="n">
+      <c r="Z11" s="20" t="n">
         <v>0.489572135024726</v>
       </c>
-      <c r="AA11" s="34" t="n">
+      <c r="AA11" s="20" t="n">
         <v>0.426657263751763</v>
       </c>
-      <c r="AB11" s="34" t="n">
+      <c r="AB11" s="20" t="n">
         <v>0.178589232303091</v>
       </c>
-      <c r="AC11" s="34" t="n">
+      <c r="AC11" s="20" t="n">
         <v>0.0391615063220045</v>
       </c>
-      <c r="AD11" s="34" t="n">
+      <c r="AD11" s="20" t="n">
         <v>0.489142119974199</v>
       </c>
-      <c r="AE11" s="34" t="n">
+      <c r="AE11" s="20" t="n">
         <v>0.437099567248307</v>
       </c>
-      <c r="AF11" s="34" t="n">
+      <c r="AF11" s="20" t="n">
         <v>0.28895</v>
       </c>
-      <c r="AG11" s="34" t="n">
+      <c r="AG11" s="20" t="n">
         <v>0.285714</v>
       </c>
-      <c r="AH11" s="34" t="n">
+      <c r="AH11" s="20" t="n">
         <v>0.306892</v>
       </c>
-      <c r="AI11" s="34" t="n">
+      <c r="AI11" s="20" t="n">
         <v>0.345525</v>
+      </c>
+      <c r="AJ11" s="20" t="n">
+        <v>0.009392</v>
+      </c>
+      <c r="AK11" s="20" t="n">
+        <v>0.455624</v>
+      </c>
+      <c r="AL11" s="20" t="n">
+        <v>0.411391</v>
+      </c>
+      <c r="AM11" s="20" t="n">
+        <v>0.407418</v>
+      </c>
+      <c r="AN11" s="20" t="n">
+        <v>0.792265</v>
+      </c>
+      <c r="AO11" s="20" t="n">
+        <v>0.757714</v>
+      </c>
+      <c r="AP11" s="20" t="n">
+        <v>0.727726</v>
+      </c>
+      <c r="AQ11" s="20" t="n">
+        <v>0.679095</v>
+      </c>
+      <c r="AR11" s="21" t="n">
+        <f aca="false">MAX(D11:AQ11)</f>
+        <v>0.792265</v>
+      </c>
+      <c r="AS11" s="21" t="n">
+        <f aca="false">MAX(D11:S11)</f>
+        <v>0.420814142033193</v>
       </c>
     </row>
     <row r="12" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>1533</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D12" s="35" t="n">
+      <c r="B12" s="19" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D12" s="20" t="n">
         <v>0.0334599933019946</v>
       </c>
-      <c r="E12" s="35" t="n">
+      <c r="E12" s="20" t="n">
         <v>0.0291193471204669</v>
       </c>
-      <c r="F12" s="35" t="n">
+      <c r="F12" s="20" t="n">
         <v>0.0283902144367261</v>
       </c>
-      <c r="G12" s="35" t="n">
+      <c r="G12" s="20" t="n">
         <v>0.534346504559271</v>
       </c>
-      <c r="H12" s="35" t="n">
+      <c r="H12" s="20" t="n">
         <v>0.067872177757416</v>
       </c>
-      <c r="I12" s="35" t="n">
+      <c r="I12" s="20" t="n">
         <v>0.0291193471204669</v>
       </c>
-      <c r="J12" s="35" t="n">
+      <c r="J12" s="20" t="n">
         <v>0.0283902144367261</v>
       </c>
-      <c r="K12" s="35" t="n">
+      <c r="K12" s="20" t="n">
         <v>0.431410883023786</v>
       </c>
-      <c r="L12" s="35" t="n">
+      <c r="L12" s="20" t="n">
         <v>0.0677915997444698</v>
       </c>
-      <c r="M12" s="35" t="n">
+      <c r="M12" s="20" t="n">
         <v>0.0291193471204669</v>
       </c>
-      <c r="N12" s="35" t="n">
+      <c r="N12" s="20" t="n">
         <v>0.0283902144367261</v>
       </c>
-      <c r="O12" s="35" t="n">
+      <c r="O12" s="20" t="n">
         <v>0.431410883023786</v>
       </c>
-      <c r="P12" s="37" t="n">
+      <c r="P12" s="20" t="n">
         <v>0.587933136280524</v>
       </c>
-      <c r="Q12" s="35" t="n">
+      <c r="Q12" s="20" t="n">
         <v>0.526353468533171</v>
       </c>
-      <c r="R12" s="35" t="n">
+      <c r="R12" s="20" t="n">
         <v>0.543722673329169</v>
       </c>
-      <c r="S12" s="35" t="n">
+      <c r="S12" s="20" t="n">
         <v>0.53677811550152</v>
       </c>
-      <c r="T12" s="35" t="n">
+      <c r="T12" s="20" t="n">
         <v>0.3807495984251</v>
       </c>
-      <c r="U12" s="35" t="n">
+      <c r="U12" s="20" t="n">
         <v>0.55374983920072</v>
       </c>
-      <c r="V12" s="35" t="n">
+      <c r="V12" s="20" t="n">
         <v>0.437594236890602</v>
       </c>
-      <c r="W12" s="35" t="n">
+      <c r="W12" s="20" t="n">
         <v>0.0535294117647059</v>
       </c>
-      <c r="X12" s="35" t="n">
+      <c r="X12" s="20" t="n">
         <v>0.3807495984251</v>
       </c>
-      <c r="Y12" s="35" t="n">
+      <c r="Y12" s="20" t="n">
         <v>0.553835598816517</v>
       </c>
-      <c r="Z12" s="35" t="n">
+      <c r="Z12" s="20" t="n">
         <v>0.437594236890602</v>
       </c>
-      <c r="AA12" s="35" t="n">
+      <c r="AA12" s="20" t="n">
         <v>0.0535294117647059</v>
       </c>
-      <c r="AB12" s="35" t="n">
+      <c r="AB12" s="20" t="n">
         <v>0.403398225649707</v>
       </c>
-      <c r="AC12" s="35" t="n">
+      <c r="AC12" s="20" t="n">
         <v>0.527846137716177</v>
       </c>
-      <c r="AD12" s="35" t="n">
+      <c r="AD12" s="20" t="n">
         <v>0.437594236890602</v>
       </c>
-      <c r="AE12" s="35" t="n">
+      <c r="AE12" s="20" t="n">
         <v>0.0250339662546097</v>
       </c>
-      <c r="AF12" s="38" t="n">
+      <c r="AF12" s="20" t="n">
         <v>0.816353</v>
       </c>
-      <c r="AG12" s="37" t="n">
+      <c r="AG12" s="20" t="n">
         <v>0.785046</v>
       </c>
-      <c r="AH12" s="37" t="n">
+      <c r="AH12" s="20" t="n">
         <v>0.7501</v>
       </c>
-      <c r="AI12" s="37" t="n">
+      <c r="AI12" s="20" t="n">
         <v>0.740256</v>
+      </c>
+      <c r="AJ12" s="20" t="n">
+        <v>0.81434</v>
+      </c>
+      <c r="AK12" s="20" t="n">
+        <v>0.780095</v>
+      </c>
+      <c r="AL12" s="20" t="n">
+        <v>0.7501</v>
+      </c>
+      <c r="AM12" s="20" t="n">
+        <v>0.740256</v>
+      </c>
+      <c r="AN12" s="20" t="n">
+        <v>0.81818</v>
+      </c>
+      <c r="AO12" s="20" t="n">
+        <v>0.78592</v>
+      </c>
+      <c r="AP12" s="20" t="n">
+        <v>0.125687</v>
+      </c>
+      <c r="AQ12" s="20" t="n">
+        <v>0.73921</v>
+      </c>
+      <c r="AR12" s="21" t="n">
+        <f aca="false">MAX(D12:AQ12)</f>
+        <v>0.81818</v>
+      </c>
+      <c r="AS12" s="21" t="n">
+        <f aca="false">MAX(D12:S12)</f>
+        <v>0.587933136280524</v>
       </c>
     </row>
     <row r="13" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>1188</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>1533</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D13" s="34" t="n">
+      <c r="B13" s="19" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D13" s="20" t="n">
         <v>0.628033319248895</v>
       </c>
-      <c r="E13" s="34" t="n">
+      <c r="E13" s="20" t="n">
         <v>0.104923798358734</v>
       </c>
-      <c r="F13" s="34" t="n">
+      <c r="F13" s="20" t="n">
         <v>0.620603015075377</v>
       </c>
-      <c r="G13" s="34" t="n">
+      <c r="G13" s="20" t="n">
         <v>0.680050847133415</v>
       </c>
-      <c r="H13" s="34" t="n">
+      <c r="H13" s="20" t="n">
         <v>0.634930085351499</v>
       </c>
-      <c r="I13" s="34" t="n">
+      <c r="I13" s="20" t="n">
         <v>0.0789652825051055</v>
       </c>
-      <c r="J13" s="34" t="n">
+      <c r="J13" s="20" t="n">
         <v>0.022005666964104</v>
       </c>
-      <c r="K13" s="34" t="n">
+      <c r="K13" s="20" t="n">
         <v>0.00550206327372765</v>
       </c>
-      <c r="L13" s="34" t="n">
+      <c r="L13" s="20" t="n">
         <v>0.634930085351499</v>
       </c>
-      <c r="M13" s="34" t="n">
+      <c r="M13" s="20" t="n">
         <v>0.0789652825051055</v>
       </c>
-      <c r="N13" s="34" t="n">
+      <c r="N13" s="20" t="n">
         <v>0.022005666964104</v>
       </c>
-      <c r="O13" s="34" t="n">
+      <c r="O13" s="20" t="n">
         <v>0.00602409638554217</v>
       </c>
-      <c r="P13" s="34" t="n">
+      <c r="P13" s="20" t="n">
         <v>0.702225948452141</v>
       </c>
-      <c r="Q13" s="34" t="n">
+      <c r="Q13" s="20" t="n">
         <v>0.718640093786635</v>
       </c>
-      <c r="R13" s="34" t="n">
+      <c r="R13" s="20" t="n">
         <v>0.731698081724074</v>
       </c>
-      <c r="S13" s="34" t="n">
+      <c r="S13" s="20" t="n">
         <v>0.709228824273072</v>
       </c>
-      <c r="T13" s="34" t="n">
+      <c r="T13" s="20" t="n">
         <v>0.0767034640274077</v>
       </c>
-      <c r="U13" s="34" t="n">
+      <c r="U13" s="20" t="n">
         <v>0.745603751465416</v>
       </c>
-      <c r="V13" s="33" t="n">
+      <c r="V13" s="20" t="n">
         <v>0.819280393590326</v>
       </c>
-      <c r="W13" s="33" t="n">
+      <c r="W13" s="20" t="n">
         <v>0.860935524652339</v>
       </c>
-      <c r="X13" s="34" t="n">
+      <c r="X13" s="20" t="n">
         <v>0.0767034640274077</v>
       </c>
-      <c r="Y13" s="34" t="n">
+      <c r="Y13" s="20" t="n">
         <v>0.745603751465416</v>
       </c>
-      <c r="Z13" s="33" t="n">
+      <c r="Z13" s="20" t="n">
         <v>0.819280393590326</v>
       </c>
-      <c r="AA13" s="33" t="n">
+      <c r="AA13" s="20" t="n">
         <v>0.860935524652339</v>
       </c>
-      <c r="AB13" s="34" t="n">
+      <c r="AB13" s="20" t="n">
         <v>0.0921793532429135</v>
       </c>
-      <c r="AC13" s="34" t="n">
+      <c r="AC13" s="20" t="n">
         <v>0.713657678780774</v>
       </c>
-      <c r="AD13" s="34" t="n">
+      <c r="AD13" s="20" t="n">
         <v>0.0282968754979974</v>
       </c>
-      <c r="AE13" s="34" t="n">
+      <c r="AE13" s="20" t="n">
         <v>0.00301204819277108</v>
       </c>
-      <c r="AF13" s="33" t="n">
+      <c r="AF13" s="20" t="n">
         <v>0.865243</v>
       </c>
-      <c r="AG13" s="36" t="n">
+      <c r="AG13" s="20" t="n">
         <v>0.885832</v>
       </c>
-      <c r="AH13" s="33" t="n">
+      <c r="AH13" s="20" t="n">
         <v>0.827883</v>
       </c>
-      <c r="AI13" s="33" t="n">
+      <c r="AI13" s="20" t="n">
         <v>0.861272</v>
+      </c>
+      <c r="AJ13" s="20" t="n">
+        <v>0.971171</v>
+      </c>
+      <c r="AK13" s="20" t="n">
+        <v>0.983458</v>
+      </c>
+      <c r="AL13" s="20" t="n">
+        <v>0.922547</v>
+      </c>
+      <c r="AM13" s="20" t="n">
+        <v>0.913313</v>
+      </c>
+      <c r="AN13" s="20" t="n">
+        <v>0.976126</v>
+      </c>
+      <c r="AO13" s="20" t="n">
+        <v>0.983458</v>
+      </c>
+      <c r="AP13" s="20" t="n">
+        <v>0.987952</v>
+      </c>
+      <c r="AQ13" s="20" t="n">
+        <v>0.991329</v>
+      </c>
+      <c r="AR13" s="21" t="n">
+        <f aca="false">MAX(D13:AQ13)</f>
+        <v>0.991329</v>
+      </c>
+      <c r="AS13" s="21" t="n">
+        <f aca="false">MAX(D13:S13)</f>
+        <v>0.731698081724074</v>
       </c>
     </row>
     <row r="14" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>1303</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>1543</v>
-      </c>
-      <c r="D14" s="34" t="n">
+      <c r="B14" s="19" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D14" s="20" t="n">
         <v>0.82740032220014</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="20" t="n">
         <v>0.689922480620155</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="20" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="G14" s="34" t="n">
+      <c r="G14" s="20" t="n">
         <v>0.806451612903226</v>
       </c>
-      <c r="H14" s="34" t="n">
+      <c r="H14" s="20" t="n">
         <v>0.846394984326019</v>
       </c>
-      <c r="I14" s="34" t="n">
+      <c r="I14" s="20" t="n">
         <v>0.434750066827052</v>
       </c>
-      <c r="J14" s="33" t="n">
+      <c r="J14" s="20" t="n">
         <v>0.925925925925926</v>
       </c>
-      <c r="K14" s="34" t="n">
+      <c r="K14" s="20" t="n">
         <v>0.806451612903226</v>
       </c>
-      <c r="L14" s="34" t="n">
+      <c r="L14" s="20" t="n">
         <v>0.844827586206896</v>
       </c>
-      <c r="M14" s="34" t="n">
+      <c r="M14" s="20" t="n">
         <v>0.506589147286822</v>
       </c>
-      <c r="N14" s="34" t="n">
+      <c r="N14" s="20" t="n">
         <v>0.925925925925926</v>
       </c>
-      <c r="O14" s="34" t="n">
+      <c r="O14" s="20" t="n">
         <v>0.806451612903226</v>
       </c>
-      <c r="P14" s="34" t="n">
+      <c r="P14" s="20" t="n">
         <v>0.838557993730407</v>
       </c>
-      <c r="Q14" s="33" t="n">
+      <c r="Q14" s="20" t="n">
         <v>0.908045977011494</v>
       </c>
-      <c r="R14" s="34" t="n">
+      <c r="R14" s="20" t="n">
         <v>0.819672131147541</v>
       </c>
-      <c r="S14" s="34" t="n">
+      <c r="S14" s="20" t="n">
         <v>0.774193548387097</v>
       </c>
-      <c r="T14" s="34" t="n">
+      <c r="T14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="U14" s="34" t="n">
+      <c r="U14" s="20" t="n">
         <v>0.32874420998456</v>
       </c>
-      <c r="V14" s="34" t="n">
+      <c r="V14" s="20" t="n">
         <v>0.0163934426229508</v>
       </c>
-      <c r="W14" s="34" t="n">
+      <c r="W14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="X14" s="34" t="n">
+      <c r="X14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="Y14" s="34" t="n">
+      <c r="Y14" s="20" t="n">
         <v>0.361082518442271</v>
       </c>
-      <c r="Z14" s="34" t="n">
+      <c r="Z14" s="20" t="n">
         <v>0.0163934426229508</v>
       </c>
-      <c r="AA14" s="34" t="n">
+      <c r="AA14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AB14" s="34" t="n">
+      <c r="AB14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AC14" s="34" t="n">
+      <c r="AC14" s="20" t="n">
         <v>0.00554022988505747</v>
       </c>
-      <c r="AD14" s="34" t="n">
+      <c r="AD14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AE14" s="34" t="n">
+      <c r="AE14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AF14" s="33" t="n">
+      <c r="AF14" s="20" t="n">
         <v>0.936968</v>
       </c>
-      <c r="AG14" s="36" t="n">
+      <c r="AG14" s="20" t="n">
         <v>0.943396</v>
       </c>
-      <c r="AH14" s="34" t="n">
+      <c r="AH14" s="20" t="n">
         <v>0.714286</v>
       </c>
-      <c r="AI14" s="34" t="n">
+      <c r="AI14" s="20" t="n">
         <v>0.970588</v>
+      </c>
+      <c r="AJ14" s="20" t="n">
+        <v>0.912106</v>
+      </c>
+      <c r="AK14" s="20" t="n">
+        <v>0.861905</v>
+      </c>
+      <c r="AL14" s="20" t="n">
+        <v>0.817391</v>
+      </c>
+      <c r="AM14" s="20" t="n">
+        <v>0.779661</v>
+      </c>
+      <c r="AN14" s="20" t="n">
+        <v>0.088136</v>
+      </c>
+      <c r="AO14" s="20" t="n">
+        <v>0.103093</v>
+      </c>
+      <c r="AP14" s="20" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="AQ14" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR14" s="21" t="n">
+        <f aca="false">MAX(D14:AQ14)</f>
+        <v>1</v>
+      </c>
+      <c r="AS14" s="21" t="n">
+        <f aca="false">MAX(D14:S14)</f>
+        <v>0.925925925925926</v>
       </c>
     </row>
     <row r="15" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>1400</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>1534</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>1535</v>
-      </c>
-      <c r="D15" s="34" t="n">
+      <c r="B15" s="19" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D15" s="20" t="n">
         <v>0.710144927536232</v>
       </c>
-      <c r="E15" s="34" t="n">
+      <c r="E15" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="33" t="n">
+      <c r="F15" s="20" t="n">
         <v>0.900311526479751</v>
       </c>
-      <c r="G15" s="35" t="n">
+      <c r="G15" s="20" t="n">
         <v>0.756705692048634</v>
       </c>
-      <c r="H15" s="34" t="n">
+      <c r="H15" s="20" t="n">
         <v>0.678108314263921</v>
       </c>
-      <c r="I15" s="34" t="n">
+      <c r="I15" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="J15" s="33" t="n">
+      <c r="J15" s="20" t="n">
         <v>0.897196261682243</v>
       </c>
-      <c r="K15" s="35" t="n">
+      <c r="K15" s="20" t="n">
         <v>0.858155677293028</v>
       </c>
-      <c r="L15" s="34" t="n">
+      <c r="L15" s="20" t="n">
         <v>0.681159420289855</v>
       </c>
-      <c r="M15" s="34" t="n">
+      <c r="M15" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="N15" s="33" t="n">
+      <c r="N15" s="20" t="n">
         <v>0.899505766062603</v>
       </c>
-      <c r="O15" s="35" t="n">
+      <c r="O15" s="20" t="n">
         <v>0.853464017776604</v>
       </c>
-      <c r="P15" s="34" t="n">
+      <c r="P15" s="20" t="n">
         <v>0.113653699466056</v>
       </c>
-      <c r="Q15" s="34" t="n">
+      <c r="Q15" s="20" t="n">
         <v>0.422270205446264</v>
       </c>
-      <c r="R15" s="34" t="n">
+      <c r="R15" s="20" t="n">
         <v>0.417445482866044</v>
       </c>
-      <c r="S15" s="35" t="n">
+      <c r="S15" s="20" t="n">
         <v>0.511467889908257</v>
       </c>
-      <c r="T15" s="34" t="n">
+      <c r="T15" s="20" t="n">
         <v>0.0450038138825324</v>
       </c>
-      <c r="U15" s="34" t="n">
+      <c r="U15" s="20" t="n">
         <v>0.652310563950536</v>
       </c>
-      <c r="V15" s="34" t="n">
+      <c r="V15" s="20" t="n">
         <v>0.00658978583196046</v>
       </c>
-      <c r="W15" s="35" t="n">
+      <c r="W15" s="20" t="n">
         <v>0.0144513567814868</v>
       </c>
-      <c r="X15" s="34" t="n">
+      <c r="X15" s="20" t="n">
         <v>0.045766590389016</v>
       </c>
-      <c r="Y15" s="34" t="n">
+      <c r="Y15" s="20" t="n">
         <v>0.652310563950536</v>
       </c>
-      <c r="Z15" s="34" t="n">
+      <c r="Z15" s="20" t="n">
         <v>0.00658978583196046</v>
       </c>
-      <c r="AA15" s="35" t="n">
+      <c r="AA15" s="20" t="n">
         <v>0.0167449347631382</v>
       </c>
-      <c r="AB15" s="34" t="n">
+      <c r="AB15" s="20" t="n">
         <v>0.0442410373760488</v>
       </c>
-      <c r="AC15" s="34" t="n">
+      <c r="AC15" s="20" t="n">
         <v>0.657386348661516</v>
       </c>
-      <c r="AD15" s="34" t="n">
+      <c r="AD15" s="20" t="n">
         <v>0.00658978583196046</v>
       </c>
-      <c r="AE15" s="35" t="n">
+      <c r="AE15" s="20" t="n">
         <v>0.00938331903284712</v>
       </c>
-      <c r="AF15" s="34" t="n">
+      <c r="AF15" s="20" t="n">
         <v>0.271903</v>
       </c>
-      <c r="AG15" s="34" t="n">
+      <c r="AG15" s="20" t="n">
         <v>0.308249</v>
       </c>
-      <c r="AH15" s="34" t="n">
+      <c r="AH15" s="20" t="n">
         <v>0.33985</v>
       </c>
-      <c r="AI15" s="35" t="n">
+      <c r="AI15" s="20" t="n">
         <v>0.427061</v>
       </c>
+      <c r="AJ15" s="20" t="n">
+        <v>0.952102</v>
+      </c>
+      <c r="AK15" s="20" t="n">
+        <v>0.945191</v>
+      </c>
+      <c r="AL15" s="20" t="n">
+        <v>0.931818</v>
+      </c>
+      <c r="AM15" s="20" t="n">
+        <v>0.887417</v>
+      </c>
+      <c r="AN15" s="20" t="n">
+        <v>0.019391</v>
+      </c>
+      <c r="AO15" s="20" t="n">
+        <v>0.020101</v>
+      </c>
+      <c r="AP15" s="20" t="n">
+        <v>0.128105</v>
+      </c>
+      <c r="AQ15" s="20" t="n">
+        <v>0.226087</v>
+      </c>
+      <c r="AR15" s="21" t="n">
+        <f aca="false">MAX(D15:AQ15)</f>
+        <v>0.952102</v>
+      </c>
+      <c r="AS15" s="21" t="n">
+        <f aca="false">MAX(D15:S15)</f>
+        <v>0.900311526479751</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="21" t="n">
+        <f aca="false">AVERAGE(D3:D15)</f>
+        <v>0.27723462318913</v>
+      </c>
+      <c r="E16" s="21" t="n">
+        <f aca="false">AVERAGE(E3:E15)</f>
+        <v>0.219055198881004</v>
+      </c>
+      <c r="F16" s="21" t="n">
+        <f aca="false">AVERAGE(F3:F15)</f>
+        <v>0.482253561459094</v>
+      </c>
+      <c r="G16" s="21" t="n">
+        <f aca="false">AVERAGE(G3:G15)</f>
+        <v>0.540833768723246</v>
+      </c>
+      <c r="H16" s="21" t="n">
+        <f aca="false">AVERAGE(H3:H15)</f>
+        <v>0.321549655974168</v>
+      </c>
+      <c r="I16" s="21" t="n">
+        <f aca="false">AVERAGE(I3:I15)</f>
+        <v>0.202354847633602</v>
+      </c>
+      <c r="J16" s="21" t="n">
+        <f aca="false">AVERAGE(J3:J15)</f>
+        <v>0.421340493605857</v>
+      </c>
+      <c r="K16" s="21" t="n">
+        <f aca="false">AVERAGE(K3:K15)</f>
+        <v>0.497528006621846</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21" t="n">
+        <f aca="false">AVERAGE(P3:P15)</f>
+        <v>0.38279855286588</v>
+      </c>
+      <c r="Q16" s="21" t="n">
+        <f aca="false">AVERAGE(Q3:Q15)</f>
+        <v>0.443284776613872</v>
+      </c>
+      <c r="R16" s="21" t="n">
+        <f aca="false">AVERAGE(R3:R15)</f>
+        <v>0.521942586006452</v>
+      </c>
+      <c r="S16" s="21" t="n">
+        <f aca="false">AVERAGE(S3:S15)</f>
+        <v>0.519269644885893</v>
+      </c>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="21"/>
+      <c r="AF16" s="21" t="n">
+        <f aca="false">AVERAGE(AF3:AF15)</f>
+        <v>0.596048</v>
+      </c>
+      <c r="AG16" s="21" t="n">
+        <f aca="false">AVERAGE(AG3:AG15)</f>
+        <v>0.601267538461538</v>
+      </c>
+      <c r="AH16" s="21" t="n">
+        <f aca="false">AVERAGE(AH3:AH15)</f>
+        <v>0.577555</v>
+      </c>
+      <c r="AI16" s="21" t="n">
+        <f aca="false">AVERAGE(AI3:AI15)</f>
+        <v>0.625131538461538</v>
+      </c>
+      <c r="AJ16" s="21" t="n">
+        <f aca="false">AVERAGE(AJ3:AJ15)</f>
+        <v>0.707155307692308</v>
+      </c>
+      <c r="AK16" s="21" t="n">
+        <f aca="false">AVERAGE(AK3:AK15)</f>
+        <v>0.714027846153846</v>
+      </c>
+      <c r="AL16" s="21" t="n">
+        <f aca="false">AVERAGE(AL3:AL15)</f>
+        <v>0.598580461538462</v>
+      </c>
+      <c r="AM16" s="21" t="n">
+        <f aca="false">AVERAGE(AM3:AM15)</f>
+        <v>0.657057153846154</v>
+      </c>
+      <c r="AN16" s="21" t="n">
+        <f aca="false">AVERAGE(AN3:AN15)</f>
+        <v>0.593061692307692</v>
+      </c>
+      <c r="AO16" s="21" t="n">
+        <f aca="false">AVERAGE(AO3:AO15)</f>
+        <v>0.578382076923077</v>
+      </c>
+      <c r="AP16" s="21" t="n">
+        <f aca="false">AVERAGE(AP3:AP15)</f>
+        <v>0.411921461538462</v>
+      </c>
+      <c r="AQ16" s="21" t="n">
+        <f aca="false">AVERAGE(AQ3:AQ15)</f>
+        <v>0.481492076923077</v>
+      </c>
+      <c r="AR16" s="21" t="n">
+        <f aca="false">MAX(D16:AQ16)</f>
+        <v>0.714027846153846</v>
+      </c>
+      <c r="AS16" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:K1"/>
@@ -18986,6 +19464,9 @@
     <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>